<commit_message>
Add and Update README
</commit_message>
<xml_diff>
--- a/inst/extdata/artesianwells.xlsx
+++ b/inst/extdata/artesianwells.xlsx
@@ -29,7 +29,7 @@
     <t xml:space="preserve">district</t>
   </si>
   <si>
-    <t xml:space="preserve">trad_auth</t>
+    <t xml:space="preserve">traditional_authority</t>
   </si>
   <si>
     <t xml:space="preserve">well_images</t>
@@ -38,19 +38,19 @@
     <t xml:space="preserve">has_structure</t>
   </si>
   <si>
-    <t xml:space="preserve">structure_type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">structure_type_other</t>
+    <t xml:space="preserve">well_structure_type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">well_structure_type_other</t>
   </si>
   <si>
     <t xml:space="preserve">can_test_flow</t>
   </si>
   <si>
-    <t xml:space="preserve">fill_time_20l</t>
-  </si>
-  <si>
-    <t xml:space="preserve">community_use</t>
+    <t xml:space="preserve">seconds_to_fill_20L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">use_of_site</t>
   </si>
   <si>
     <t xml:space="preserve">other_site_use</t>

</xml_diff>